<commit_message>
feat: upload consultant photos and update team Excel with URLs
Add profile photos for Marnix, Noud and Rick to data/. Upload images
to Catbox.moe and store the resulting URLs in the Foto-URL column of
ai-panda-team.xlsx (rows 12-14). Rebuild plugin ZIP to include updated
Excel.

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/ai-panda-team.xlsx
+++ b/data/ai-panda-team.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marnix/Documents/Projecten/Ai Panda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marnix/Documents/Projecten/Ai Panda Klantpagina/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA3D155D-9E0F-B945-AAF0-81489A536163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1284443E-8F16-2745-ACCE-EC632A89F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="660" windowWidth="29280" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="AI Panda Team" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AI Panda Team'!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AI Panda Team'!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Naam</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Functie</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
     <t>Foto-URL</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>Co-Founder / Consultant</t>
   </si>
   <si>
-    <t>Kernteam</t>
-  </si>
-  <si>
     <t>jack@aipanda.nl</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>Customer Impact Lead</t>
   </si>
   <si>
-    <t>AIXcellerator</t>
-  </si>
-  <si>
     <t>stephan@aipanda.nl</t>
   </si>
   <si>
@@ -133,12 +124,24 @@
     <t>Marnix</t>
   </si>
   <si>
+    <t>https://files.catbox.moe/3zpxbt.png</t>
+  </si>
+  <si>
+    <t>06-26883024</t>
+  </si>
+  <si>
     <t>marnix@aipanda.nl</t>
   </si>
   <si>
     <t>Noud</t>
   </si>
   <si>
+    <t>https://files.catbox.moe/hj7s40.png</t>
+  </si>
+  <si>
+    <t>06-47920832</t>
+  </si>
+  <si>
     <t>noud@aipanda.nl</t>
   </si>
   <si>
@@ -148,10 +151,7 @@
     <t>Ai Consultant</t>
   </si>
   <si>
-    <t>06-26883024</t>
-  </si>
-  <si>
-    <t>06-47920832</t>
+    <t>https://files.catbox.moe/vcp4cq.png</t>
   </si>
   <si>
     <t>06-34287409</t>
@@ -251,7 +251,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -273,7 +273,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -580,24 +580,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,218 +612,194 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="F12" r:id="rId1" xr:uid="{4C208F0A-C194-F94D-85EC-A6A7CBD6FCE6}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{3844C291-7DDA-BD4B-AB21-F0C9FA334AF8}"/>
-    <hyperlink ref="F14" r:id="rId3" xr:uid="{410A36C8-E93D-9147-89BB-8B14DCD71BC2}"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: correct Notion markdown syntax in skill templates
Replace invalid <callout> HTML tags with Pandoc-style fenced divs,
fix column children indentation, remove image captions from team
photos, remove non-existent <embed> tag, and update Gemini model
to gemini-3-pro-image-preview everywhere.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/ai-panda-team.xlsx
+++ b/data/ai-panda-team.xlsx
@@ -783,7 +783,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://files.catbox.moe/3zpxbt.png</t>
+          <t>https://0x0.st/PuWR.png</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://files.catbox.moe/hj7s40.png</t>
+          <t>https://0x0.st/PuW7.png</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://files.catbox.moe/vcp4cq.png</t>
+          <t>https://0x0.st/PuWh.png</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">

</xml_diff>